<commit_message>
Progression chapitre 5 Lidar
</commit_message>
<xml_diff>
--- a/SuiviTodo.xlsx
+++ b/SuiviTodo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="4600" windowWidth="16000" windowHeight="10300" tabRatio="500"/>
+    <workbookView xWindow="7920" yWindow="2940" windowWidth="16000" windowHeight="10300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -107,7 +106,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Feuil1!$C$4</c:f>
@@ -120,6 +121,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -129,19 +131,28 @@
               <c:f>Feuil1!$B$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>09/08/18</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Feuil1!$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>120.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -154,7 +165,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Feuil1!$C$6</c:f>
@@ -164,6 +177,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -176,7 +190,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Feuil1!$C$7</c:f>
@@ -186,6 +202,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -198,7 +215,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Feuil1!$C$8</c:f>
@@ -208,6 +227,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -220,7 +240,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:val>
             <c:numRef>
               <c:f>Feuil1!$C$9</c:f>
@@ -230,6 +252,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -239,13 +262,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="2089053704"/>
-        <c:axId val="2089091384"/>
-      </c:barChart>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2080065384"/>
+        <c:axId val="2080067624"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="2089053704"/>
+        <c:axId val="2080065384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -254,7 +277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089091384"/>
+        <c:crossAx val="2080067624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -262,7 +285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089091384"/>
+        <c:axId val="2080067624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -273,7 +296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2089053704"/>
+        <c:crossAx val="2080065384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -652,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -679,6 +702,14 @@
         <v>144</v>
       </c>
     </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1">
+        <v>43321</v>
+      </c>
+      <c r="C5">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Localisation kalman theo ok + attitudes 3D
</commit_message>
<xml_diff>
--- a/SuiviTodo.xlsx
+++ b/SuiviTodo.xlsx
@@ -162,6 +162,9 @@
               <c:f>Feuil1!$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20/08/18</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -174,6 +177,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>124.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -187,6 +193,9 @@
               <c:f>Feuil1!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21/08/18</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -199,6 +208,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>126.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -264,11 +276,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2080065384"/>
-        <c:axId val="2080067624"/>
+        <c:axId val="2107158360"/>
+        <c:axId val="2107161544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2080065384"/>
+        <c:axId val="2107158360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -277,7 +289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080067624"/>
+        <c:crossAx val="2107161544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -285,7 +297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080067624"/>
+        <c:axId val="2107161544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -296,7 +308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080065384"/>
+        <c:crossAx val="2107158360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -675,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -708,6 +720,22 @@
       </c>
       <c r="C5">
         <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="1">
+        <v>43332</v>
+      </c>
+      <c r="C6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="1">
+        <v>43333</v>
+      </c>
+      <c r="C7">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>